<commit_message>
initial results + plots of 3Js
</commit_message>
<xml_diff>
--- a/Interleaved-Christian/evap_N_circ_cross_couter_flow/tuning_exp.xlsx
+++ b/Interleaved-Christian/evap_N_circ_cross_couter_flow/tuning_exp.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Desktop\Test\Interleaved-Christian\evap_N_circ_cross_couter_flow\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="345" windowWidth="25725" windowHeight="14850"/>
+    <workbookView xWindow="0" yWindow="690" windowWidth="25725" windowHeight="14850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>baseline</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>T_a</t>
+  </si>
+  <si>
+    <t>T_sup</t>
   </si>
 </sst>
 </file>
@@ -411,15 +414,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E2" sqref="E2:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,8 +435,11 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -446,8 +452,11 @@
       <c r="D2">
         <v>13.03</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>15.91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -460,8 +469,11 @@
       <c r="D3">
         <v>15.35</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>13.64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -474,8 +486,11 @@
       <c r="D4">
         <v>12.12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>15.83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -488,8 +503,11 @@
       <c r="D5">
         <v>12.78</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>15.55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -502,8 +520,11 @@
       <c r="D6">
         <v>16.41</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>12.78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -516,8 +537,11 @@
       <c r="D7">
         <v>16.36</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>13.66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -530,8 +554,11 @@
       <c r="D8">
         <v>17.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>12.47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -543,6 +570,9 @@
       </c>
       <c r="D9">
         <v>21.34</v>
+      </c>
+      <c r="E9">
+        <v>11.42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>